<commit_message>
solucione el error de que se generen dos BDD iguales
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -1,40 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92f6345f5ffe4c96/PROGRAMACION/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59C097555AD1A7FAAE1593431510344D078EFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{384A1B5E-4FE9-408F-8C0E-3F3143AB92E1}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Capacidad</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -66,82 +96,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -429,142 +401,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col width="21.5703125" customWidth="1" min="1" max="1"/>
-    <col width="19.28515625" customWidth="1" min="2" max="2"/>
-    <col width="27.140625" customWidth="1" min="3" max="3"/>
+    <col min="1" max="1" width="7.77734375" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Usuario</t>
-        </is>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Contraseña</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Tipo</t>
-        </is>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>333</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>333</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>rosana</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>emanuel</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ema</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>igna</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modificamos la pantalla restaurante poniendo los botones
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92f6345f5ffe4c96/PROGRAMACION/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92f6345f5ffe4c96/Programacion I/PROGRAMACION  TP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59C097555AD1A7FAAE1593431510344D078EFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{384A1B5E-4FE9-408F-8C0E-3F3143AB92E1}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_2B59C097555AD1A7FAAE1593431510344D078EFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D747E47-A430-40AF-81B1-539699A784D2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,8 +410,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
agregue el boto nde lahistoria del restaurante (chiche)
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -1,63 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92f6345f5ffe4c96/Programacion I/PROGRAMACION  TP/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_2B59C097555AD1A7FAAE1593431510344D078EFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D747E47-A430-40AF-81B1-539699A784D2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Capacidad</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -97,23 +75,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -401,37 +438,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col width="13.44140625" customWidth="1" min="1" max="1"/>
+    <col width="11.44140625" customWidth="1" min="2" max="2"/>
+    <col width="13.21875" customWidth="1" min="3" max="3"/>
+    <col width="12.44140625" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Capacidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11">
+      <c r="H11" s="2" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H11" s="2"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
agregue las mesas, funcionalidades de agregar, eliminar, modificar, reservar, cancelar reserva, validaciones de si entra alguien a querer reservar una mesa reservada, vincule con la bdd,el admin modifica la cantidad desocupa o elimina, agrega con la capacidad correspondiente
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -513,26 +513,28 @@
           <t>Libre</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>4</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>3</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -540,7 +542,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -552,21 +554,40 @@
           <t>Libre</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>5</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t>Libre</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
         <v>8</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambie el entry de la reserva para que soloo aparezca reservar y el boton diga el nombre del usuario
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -16,20 +16,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -74,10 +66,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,10 +434,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -479,114 +470,34 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11">
-      <c r="H11" s="2" t="n"/>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" t="inlineStr">
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
         <is>
           <t>Libre</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>2</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>4</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>6</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>5</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>7</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>8</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
cuando esta reservada y quiero cancelar ya no aparece el boton reservar otra vez y ahora el cancelar reserva esta arriba del boton atras, esos cambios hice
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -434,10 +434,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D4" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -472,7 +472,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -487,15 +487,45 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr"/>
+        <v>3</v>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>Libre</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>4</t>
         </is>

</xml_diff>

<commit_message>
pusimos la imagen nueva y la función redimensionar, cambiamos tipos de letras, colores de fondo y de botones, pusimos para poder cambiar numero de mesa, validamos que si no tiene las imágenes el sistema funciona igual, separamos un poco las mesas, sacamos el entry para que no usen nombres falsos para reservar, separe el codigo por secciones para que no quede todo en un mismo .py
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="A2:D4"/>
@@ -519,7 +519,6 @@
       <c r="A5" t="n">
         <v>1</v>
       </c>
-      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -528,6 +527,37 @@
       <c r="D5" t="inlineStr">
         <is>
           <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
limpie todos los datos de las bdd
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -1,40 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92f6345f5ffe4c96/Programacion I/PROGRAMACION  TP/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_2B59C097559ADE6AC8BCDF304C1510344D078E56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6C5F785-E6FF-4FD4-991F-7E9C8596441B}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Capacidad</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -67,81 +94,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -429,136 +397,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="A2:D4"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="13.44140625" customWidth="1" min="1" max="1"/>
-    <col width="11.44140625" customWidth="1" min="2" max="2"/>
-    <col width="13.21875" customWidth="1" min="3" max="3"/>
-    <col width="12.44140625" customWidth="1" min="4" max="4"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Usuario</t>
-        </is>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Capacidad</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>6</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>7</v>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Libre</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
guardo lo que probe para que si esta resrvada la mesa aparezca otra imagen
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -1,60 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/92f6345f5ffe4c96/Programacion I/PROGRAMACION  TP/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2B59C097559ADE6AC8BCDF304C1510344D078E56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6C5F785-E6FF-4FD4-991F-7E9C8596441B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Capacidad</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -94,22 +67,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -397,27 +429,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Capacidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ocupada</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>3</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dividi la interfaz restaurante para poner los botones en u ncostado y el restaurante del otro, le di relieves a los botones
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="A2:D2"/>
@@ -468,14 +468,9 @@
       <c r="A2" t="n">
         <v>2</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ocupada</t>
+          <t>Libre</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -493,6 +488,35 @@
       </c>
       <c r="D3" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saque el for que hacia que siempre hayan 9 mesas, si no existe bdd se hacen las 9 y si existe el excel se basa en las mesas que estan cargadas ahi, y si se borra una mesa al agregar toma el lugar de la que se elimino ya que el excel deja un espacio vacio y al agregar la mesa recorre el excel si hay lugar vacio usa ese sino toma el numero de mesas que hay y se pone en el siguiente (+1)
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -25,21 +26,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -47,31 +42,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -434,31 +413,31 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Usuario</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Capacidad</t>
         </is>
@@ -466,8 +445,9 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -479,8 +459,9 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -492,8 +473,9 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -505,7 +487,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
@@ -513,10 +495,78 @@
           <t>Libre</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Libre</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modificó la distribución de mesas para usar posiciones fijas en grid. Antes las mesas se autoacomodaban automáticamente según el espacio disponible, pero ahora se definieron posiciones manuales, lo que provoca que queden huecos en la grilla cuando no todas las posiciones están ocupadas.
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -447,7 +447,6 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -461,7 +460,6 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -475,7 +473,6 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -489,7 +486,6 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -501,9 +497,8 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr"/>
+        <v>6</v>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -515,9 +510,8 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr"/>
+        <v>7</v>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -529,9 +523,8 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr"/>
+        <v>8</v>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -543,9 +536,8 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr"/>
+        <v>9</v>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>Libre</t>
@@ -557,16 +549,17 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr"/>
+        <v>5</v>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>Libre</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>4</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregue la validacion de si la mesa esta reservada el admin no la puede borrar
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -512,9 +512,14 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Libre</t>
+          <t>Ocupada</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -525,7 +530,6 @@
       <c r="A8" t="n">
         <v>8</v>
       </c>
-      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
           <t>Libre</t>

</xml_diff>

<commit_message>
agrande todas las pantallas para que esten del mismo tamaño
</commit_message>
<xml_diff>
--- a/Datos_Reservas.xlsx
+++ b/Datos_Reservas.xlsx
@@ -512,14 +512,10 @@
       <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ocupada</t>
+          <t>Libre</t>
         </is>
       </c>
       <c r="D7" t="n">

</xml_diff>